<commit_message>
code comments and updates
</commit_message>
<xml_diff>
--- a/session_2_dice_music/markovChainDrum/drawMatrix.xlsx
+++ b/session_2_dice_music/markovChainDrum/drawMatrix.xlsx
@@ -165,8 +165,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -216,7 +220,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -227,6 +231,8 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -237,6 +243,8 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,7 +577,7 @@
   <dimension ref="A3:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>